<commit_message>
updated metabolights assay for reviewing
</commit_message>
<xml_diff>
--- a/templates/3ASY03_MetabolomicsMassSpec/3ASY03_MetabolomicsMassSpec.xlsx
+++ b/templates/3ASY03_MetabolomicsMassSpec/3ASY03_MetabolomicsMassSpec.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\3ASY03_MetabolomicsMassSpec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FE846D-86CB-4259-8286-A0290A6DB399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B57057-18F0-4DD6-BF76-3D83B18FB252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A3B5FB5-5846-1147-AD66-144B0B2820ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="227">
   <si>
     <t>Source Name</t>
   </si>
@@ -570,13 +570,163 @@
   </si>
   <si>
     <t>The name of the input (the source) of this assay.</t>
+  </si>
+  <si>
+    <t>A: H2O (0.1% formic acid), B: ACN (0.1% formic acid)</t>
+  </si>
+  <si>
+    <t>20% ACN</t>
+  </si>
+  <si>
+    <t>Parameter [mobile phase]</t>
+  </si>
+  <si>
+    <t>mobile phase</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHMO_0000995</t>
+  </si>
+  <si>
+    <t>CHMO:0000995</t>
+  </si>
+  <si>
+    <t>Parameter [elution]</t>
+  </si>
+  <si>
+    <t>gradient elution</t>
+  </si>
+  <si>
+    <t>isocratic elution</t>
+  </si>
+  <si>
+    <t>elution</t>
+  </si>
+  <si>
+    <t>CHMO:0002742</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHMO_0002742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you can also describe your gradient </t>
+  </si>
+  <si>
+    <t>EXTRACTION - Derivatization</t>
+  </si>
+  <si>
+    <t>If the sample has been subjected to chemical modification prior to injection.</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>CHROMATOGRAPHY - Chromatography Instrument</t>
+  </si>
+  <si>
+    <t>Add the full name of the instrument you used for the Chromatographic part of this assay, including the manufacturer and model number as reported in manufacturer’s brochures, user manuals, or on their website.</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>CHROMATOGRAPHY - Column Model</t>
+  </si>
+  <si>
+    <t>Manufacturer, model number and dimensions in the format shown in the examples:</t>
+  </si>
+  <si>
+    <t>Parameter [label]</t>
+  </si>
+  <si>
+    <t>13C</t>
+  </si>
+  <si>
+    <t>15N</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_35209</t>
+  </si>
+  <si>
+    <t>CHEBI:35209</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>CHROMATOGRAPHY - Label</t>
+  </si>
+  <si>
+    <t>If you used a chemical or biochemical marker in the sample such as a radioactive isotope of fluorescent dye which is bound to a material in order to make it detectable in an analytical instrument then enter it here.</t>
+  </si>
+  <si>
+    <t>MASS SPECTROMETRY - Scan Polarity</t>
+  </si>
+  <si>
+    <t>This should be ‘positive’ for a GC/MS assay. If you performed a LC/MS assay, values should identical within each assay. If you have ‘positive’ or ‘negative’ values in the same assay then split them into separate ‘positive’ and ‘negative’ assays.</t>
+  </si>
+  <si>
+    <t>MASS SPECTROMETRY - Scan m/z Range</t>
+  </si>
+  <si>
+    <t>The range used in the assay.</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>MASS SPECTROMETRY - Instrument</t>
+  </si>
+  <si>
+    <t>Add the full name of the mass spectrometer/detector you used for this assay, including the instrument manufacturer and model number as reported in manufacturer’s brochures, user manuals, or on their website.</t>
+  </si>
+  <si>
+    <t>MASS SPECTROMETRY - Ion Source</t>
+  </si>
+  <si>
+    <t>Where applicable to the instrument.</t>
+  </si>
+  <si>
+    <t>MASS SPECTROMETRY - Mass Analyzer</t>
+  </si>
+  <si>
+    <t>The analyser/detector of the mass fragments generated during the assay,</t>
+  </si>
+  <si>
+    <t>MASS SPECTROMETRY - MS Assay Name</t>
+  </si>
+  <si>
+    <t>This can be, but doesn’t have to be, the same as the ‘Sample Name’</t>
+  </si>
+  <si>
+    <t>Term Source REF [label] (#h; #tNFDI4PSO:0000079)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [label] (#h; #tNFDI4PSO:0000079)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [mobile phase] (#h; #tNFDI4PSO:0000080)</t>
+  </si>
+  <si>
+    <t>Term Source REF [mobile phase] (#h; #tNFDI4PSO:0000080)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [elution] (#h; #tNFDI4PSO:0000081)</t>
+  </si>
+  <si>
+    <t>Term Source REF [elution] (#h; #tNFDI4PSO:0000081)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -646,6 +796,17 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -742,7 +903,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,13 +1020,34 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{751FC18E-D306-8B42-912B-598F45328FEF}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -928,57 +1110,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2BA91F90-A206-C24A-B071-E1351392860E}" name="annotationTable" displayName="annotationTable" ref="D2:BA3" totalsRowShown="0">
-  <autoFilter ref="D2:BA3" xr:uid="{155D8245-62B7-F340-A809-633676FF14D5}"/>
-  <tableColumns count="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2BA91F90-A206-C24A-B071-E1351392860E}" name="annotationTable" displayName="annotationTable" ref="D2:BJ3" totalsRowShown="0">
+  <autoFilter ref="D2:BJ3" xr:uid="{155D8245-62B7-F340-A809-633676FF14D5}"/>
+  <tableColumns count="59">
     <tableColumn id="1" xr3:uid="{BBBF64BA-87C6-D34E-A6CD-4299F4D962C8}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{14AC94B4-25B3-E44B-8B75-F5DA7ADF4505}" name="Sample Name"/>
-    <tableColumn id="3" xr3:uid="{DE8A40D7-A9A3-6D44-A444-4CDA584115FB}" name="Parameter [MS sample post-extraction]" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{DE8A40D7-A9A3-6D44-A444-4CDA584115FB}" name="Parameter [MS sample post-extraction]" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{91DB6965-9407-084F-B87C-167B363C8F64}" name="Term Source REF [MS sample post-extraction] (#h; #tNFDI4PSO:0000043)"/>
     <tableColumn id="5" xr3:uid="{8F068F1B-0799-934A-A950-0CCA864FA729}" name="Term Accession Number [MS sample post-extraction] (#h; #tNFDI4PSO:0000043)"/>
-    <tableColumn id="6" xr3:uid="{C6859ADD-6217-6046-B9CE-0E2C44AEB18F}" name="Parameter [MS sample resuspension]" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{C6859ADD-6217-6046-B9CE-0E2C44AEB18F}" name="Parameter [MS sample resuspension]" dataDxfId="17"/>
     <tableColumn id="7" xr3:uid="{7FBCD097-8CAE-F140-921C-B77023BC4AE2}" name="Term Source REF [MS sample resuspension] (#h; #tNFDI4PSO:0000044)"/>
     <tableColumn id="8" xr3:uid="{81B6A235-8405-DD4A-8C68-E37AC0D99B1B}" name="Term Accession Number [MS sample resuspension] (#h; #tNFDI4PSO:0000044)"/>
-    <tableColumn id="9" xr3:uid="{0D61368D-553F-1949-B1E3-71D3E20AD860}" name="Parameter [MS sample type]" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{0D61368D-553F-1949-B1E3-71D3E20AD860}" name="Parameter [MS sample type]" dataDxfId="16"/>
     <tableColumn id="10" xr3:uid="{6179952F-0BCA-CF4E-944F-EB19C4832C67}" name="Term Source REF [MS sample type] (#h; #tNFDI4PSO:0000045)"/>
     <tableColumn id="11" xr3:uid="{994D6D0B-5285-DE4E-95A4-E184360E374C}" name="Term Accession Number [MS sample type] (#h; #tNFDI4PSO:0000045)"/>
-    <tableColumn id="12" xr3:uid="{B56199D0-4A72-9A48-A183-6470EDD554B1}" name="Parameter [MS derivatization]" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{B56199D0-4A72-9A48-A183-6470EDD554B1}" name="Parameter [MS derivatization]" dataDxfId="15"/>
     <tableColumn id="13" xr3:uid="{2D30CB05-A2E2-F747-B469-07C250031A33}" name="Term Source REF [MS derivatization] (#h; #tNFDI4PSO:0000052)"/>
     <tableColumn id="14" xr3:uid="{6110C472-0713-954C-9FD7-812784023EE1}" name="Term Accession Number [MS derivatization] (#h; #tNFDI4PSO:0000052)"/>
-    <tableColumn id="18" xr3:uid="{F21D0BDF-9000-5547-AD8A-1BE6C6EB09E6}" name="Parameter [Chromatography instrument model]" dataDxfId="11"/>
+    <tableColumn id="51" xr3:uid="{554B6563-D38B-46C3-A7D4-BF17E7735C26}" name="Parameter [label]" dataDxfId="2"/>
+    <tableColumn id="55" xr3:uid="{0D4DB16D-2B55-49F2-B11B-157D5B2B9BFE}" name="Term Source REF [label] (#h; #tNFDI4PSO:0000079)"/>
+    <tableColumn id="59" xr3:uid="{078026AD-3C19-4E75-9D4B-210B925CD75D}" name="Term Accession Number [label] (#h; #tNFDI4PSO:0000079)"/>
+    <tableColumn id="18" xr3:uid="{F21D0BDF-9000-5547-AD8A-1BE6C6EB09E6}" name="Parameter [Chromatography instrument model]" dataDxfId="14"/>
     <tableColumn id="19" xr3:uid="{93F305FB-AF63-0547-9A9E-9316392B763C}" name="Term Source REF [Chromatography instrument model] (#h; #tNFDI4PSO:0000046)"/>
     <tableColumn id="20" xr3:uid="{036AA641-2BC0-5847-B2EF-7FA1822B2E7C}" name="Term Accession Number [Chromatography instrument model] (#h; #tNFDI4PSO:0000046)"/>
-    <tableColumn id="21" xr3:uid="{81B5AB82-D2E2-C740-93BA-2766BD270F4C}" name="Parameter [Chromatography autosampler model]" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{81B5AB82-D2E2-C740-93BA-2766BD270F4C}" name="Parameter [Chromatography autosampler model]" dataDxfId="13"/>
     <tableColumn id="22" xr3:uid="{9B4B8450-0F52-524D-BC1F-8E8E4F80A6BE}" name="Term Source REF [Chromatography autosampler model] (#h; #tNFDI4PSO:0000047)"/>
     <tableColumn id="23" xr3:uid="{2C883FF4-82A2-EF44-8B01-97DEF7569A6D}" name="Term Accession Number [Chromatography autosampler model] (#h; #tNFDI4PSO:0000047)"/>
-    <tableColumn id="24" xr3:uid="{512E4A1B-6AF1-BB4D-8962-A4698189D07B}" name="Parameter [Chromatography column type]" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{512E4A1B-6AF1-BB4D-8962-A4698189D07B}" name="Parameter [Chromatography column type]" dataDxfId="12"/>
     <tableColumn id="25" xr3:uid="{B270572B-8B22-1B4F-9EC7-50CCCD074C18}" name="Term Source REF [Chromatography column type] (#h; #tNFDI4PSO:0000053)"/>
     <tableColumn id="26" xr3:uid="{FD917BD1-F453-8F4C-BBB1-50D7883F34ED}" name="Term Accession Number [Chromatography column type] (#h; #tNFDI4PSO:0000053)"/>
-    <tableColumn id="15" xr3:uid="{B77278E7-9132-F84E-8F09-B3C5A6FCEB98}" name="Parameter [Chromatography column model]" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{B77278E7-9132-F84E-8F09-B3C5A6FCEB98}" name="Parameter [Chromatography column model]" dataDxfId="11"/>
     <tableColumn id="16" xr3:uid="{C8D2A8BF-92D3-8844-B3A5-624551FA014E}" name="Term Source REF [Chromatography column model] (#h; #tNFDI4PSO:0000048)"/>
     <tableColumn id="17" xr3:uid="{1DBC3227-CDE2-F448-A105-909606EBE21D}" name="Term Accession Number [Chromatography column model] (#h; #tNFDI4PSO:0000048)"/>
-    <tableColumn id="27" xr3:uid="{17F7E68D-3B88-FF43-A4B3-399DCFB2F59B}" name="Parameter [Chromatography guard column model]" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{17F7E68D-3B88-FF43-A4B3-399DCFB2F59B}" name="Parameter [Chromatography guard column model]" dataDxfId="10"/>
     <tableColumn id="28" xr3:uid="{A4809FDB-124E-3C42-BAE1-11373D15BF08}" name="Term Source REF [Chromatography guard column model] (#h; #tNFDI4PSO:0000049)"/>
     <tableColumn id="29" xr3:uid="{FA85BE75-6B6C-7140-AC46-8BA24514D954}" name="Term Accession Number [Chromatography guard column model] (#h; #tNFDI4PSO:0000049)"/>
-    <tableColumn id="30" xr3:uid="{183360A2-948E-BB46-9A5B-9314170BA82F}" name="Parameter [scan polarity]" dataDxfId="6"/>
+    <tableColumn id="61" xr3:uid="{91FBB916-95C1-4130-99F9-3C605D462F08}" name="Parameter [mobile phase]" dataDxfId="1"/>
+    <tableColumn id="62" xr3:uid="{5F39373C-7B4A-419A-A832-D442EDFF6D75}" name="Term Source REF [mobile phase] (#h; #tNFDI4PSO:0000080)"/>
+    <tableColumn id="63" xr3:uid="{9455D16F-3EE2-436E-B377-9A561EBF3A05}" name="Term Accession Number [mobile phase] (#h; #tNFDI4PSO:0000080)"/>
+    <tableColumn id="64" xr3:uid="{516D4528-3375-4A12-832E-AA36EF0EDBC1}" name="Parameter [elution]" dataDxfId="0"/>
+    <tableColumn id="65" xr3:uid="{958983F7-D491-4988-AE0B-A0A895FEFA61}" name="Term Source REF [elution] (#h; #tNFDI4PSO:0000081)"/>
+    <tableColumn id="66" xr3:uid="{A75D43C8-D402-4832-B200-1037B0DBB096}" name="Term Accession Number [elution] (#h; #tNFDI4PSO:0000081)"/>
+    <tableColumn id="30" xr3:uid="{183360A2-948E-BB46-9A5B-9314170BA82F}" name="Parameter [scan polarity]" dataDxfId="9"/>
     <tableColumn id="31" xr3:uid="{8CE758DF-293A-5B43-8923-E07BBEA300B9}" name="Term Source REF [scan polarity] (#h; #tMS:1000465)"/>
     <tableColumn id="32" xr3:uid="{C2D1CF91-64E8-8844-B84E-0198C9EBC687}" name="Term Accession Number [scan polarity] (#h; #tMS:1000465)"/>
-    <tableColumn id="33" xr3:uid="{1BE5C769-A04D-F344-AF0D-86BBBDED416E}" name="Parameter [scan window lower limit]" dataDxfId="5"/>
+    <tableColumn id="33" xr3:uid="{1BE5C769-A04D-F344-AF0D-86BBBDED416E}" name="Parameter [scan window lower limit]" dataDxfId="8"/>
     <tableColumn id="34" xr3:uid="{720A408D-0D3D-5A47-9C32-FA091FF2BBA5}" name="Term Source REF [scan window lower limit] (#h; #tMS:1000501)"/>
     <tableColumn id="35" xr3:uid="{10AC5530-C162-4F4B-B33D-69144D995141}" name="Term Accession Number [scan window lower limit] (#h; #tMS:1000501)"/>
-    <tableColumn id="36" xr3:uid="{C8558B98-C98A-A244-A439-51E3B9875A8F}" name="Parameter [scan window upper limit]" dataDxfId="4"/>
+    <tableColumn id="36" xr3:uid="{C8558B98-C98A-A244-A439-51E3B9875A8F}" name="Parameter [scan window upper limit]" dataDxfId="7"/>
     <tableColumn id="37" xr3:uid="{8001FAB7-F714-324C-B592-D83361B52D1A}" name="Term Source REF [scan window upper limit] (#h; #tMS:1000500)"/>
     <tableColumn id="38" xr3:uid="{09050567-9154-5644-9F7E-7A35F81C36C5}" name="Term Accession Number [scan window upper limit] (#h; #tMS:1000500)"/>
-    <tableColumn id="39" xr3:uid="{7C0DFAF7-046E-534F-9C57-89FEE3E72208}" name="Parameter [instrument model]" dataDxfId="3"/>
+    <tableColumn id="39" xr3:uid="{7C0DFAF7-046E-534F-9C57-89FEE3E72208}" name="Parameter [instrument model]" dataDxfId="6"/>
     <tableColumn id="40" xr3:uid="{3B19E320-D898-6947-A400-B7D35D58F1A6}" name="Term Source REF [instrument model] (#h; #tMS:1000031)"/>
     <tableColumn id="41" xr3:uid="{14CC0697-3DFB-3447-B1FD-767F08108295}" name="Term Accession Number [instrument model] (#h; #tMS:1000031)"/>
-    <tableColumn id="42" xr3:uid="{97CC8885-D3E6-AA4E-A1AA-E031764C9196}" name="Parameter [ionization type]" dataDxfId="2"/>
+    <tableColumn id="42" xr3:uid="{97CC8885-D3E6-AA4E-A1AA-E031764C9196}" name="Parameter [ionization type]" dataDxfId="5"/>
     <tableColumn id="43" xr3:uid="{5BD69720-0711-3440-BFAD-856D20CC0859}" name="Term Source REF [ionization type] (#h; #tMS:1000008)"/>
     <tableColumn id="44" xr3:uid="{ED78172F-0957-0649-9712-53DC91AAEF41}" name="Term Accession Number [ionization type] (#h; #tMS:1000008)"/>
-    <tableColumn id="45" xr3:uid="{209174F2-9485-7D4F-9577-999720963CA1}" name="Parameter [mass analyzer type]" dataDxfId="1"/>
+    <tableColumn id="45" xr3:uid="{209174F2-9485-7D4F-9577-999720963CA1}" name="Parameter [mass analyzer type]" dataDxfId="4"/>
     <tableColumn id="46" xr3:uid="{E1C36D22-2A7B-F04A-AF75-00C1C8C9CAF4}" name="Term Source REF [mass analyzer type] (#h; #tMS:1000443)"/>
     <tableColumn id="47" xr3:uid="{F695DECA-D1D9-A542-8FEF-479135275C4A}" name="Term Accession Number [mass analyzer type] (#h; #tMS:1000443)"/>
-    <tableColumn id="48" xr3:uid="{B0DDCF73-7408-C247-9E67-7CBF0B943A49}" name="Parameter [detector type]" dataDxfId="0"/>
+    <tableColumn id="48" xr3:uid="{B0DDCF73-7408-C247-9E67-7CBF0B943A49}" name="Parameter [detector type]" dataDxfId="3"/>
     <tableColumn id="49" xr3:uid="{9E7C28E6-2B09-5A4D-BEA2-E89CA9B02622}" name="Term Source REF [detector type] (#h; #tMS:1000026)"/>
     <tableColumn id="50" xr3:uid="{2EAE4DF7-6E4D-8044-9A56-E7115F15BB64}" name="Term Accession Number [detector type] (#h; #tMS:1000026)"/>
   </tableColumns>
@@ -1283,7 +1474,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="597" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1301,13 +1492,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35F31B6-C4E7-AF4A-AFC7-8DE959780CB6}">
-  <dimension ref="A1:BA30"/>
+  <dimension ref="A1:BJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1315,60 +1506,69 @@
     <col min="1" max="1" width="32.5" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5" style="14"/>
-    <col min="4" max="4" width="14.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.375" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.875" style="14" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="72" style="14" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="36" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.875" style="14" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="70" style="14" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="27.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="56.625" style="14" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="62.875" style="14" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="40.375" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="57.875" style="14" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="64" style="14" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="46.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="72.625" style="14" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="78.875" style="14" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="46.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="74" style="14" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="80.125" style="14" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="40.375" style="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="68" style="14" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="74.125" style="14" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="52.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="69.5" style="14" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="75.875" style="14" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="67" style="14" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="74.875" style="14" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="81.125" style="14" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="47.625" style="14" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="53.875" style="14" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="57.625" style="14" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="63.875" style="14" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="57.625" style="14" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="63.875" style="14" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="52" style="14" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="58.125" style="14" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="49.375" style="14" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="55.625" style="14" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="53.375" style="14" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="59.5" style="14" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="37.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="48.125" style="14" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="54.375" style="14" hidden="1" customWidth="1"/>
-    <col min="54" max="16384" width="37.5" style="14"/>
+    <col min="4" max="4" width="42.75" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.125" style="14" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="73.875" style="14" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="38" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.25" style="14" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="72" style="14" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="28.375" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="57.625" style="14" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="64.375" style="14" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="42.75" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="58.875" style="14" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="65.75" style="14" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="40.125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="47.75" style="14" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="54.625" style="14" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="49.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="75" style="14" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="81.75" style="14" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="49.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="76.125" style="14" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="83" style="14" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="42.75" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="69.875" style="14" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="76.75" style="14" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="64.25" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="71.5" style="14" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="78.25" style="14" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="68.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="77" style="14" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="83.75" style="14" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="46.375" style="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="55.5" style="14" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="62.125" style="14" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="42.75" style="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="53.125" style="14" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="60" style="14" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="48.625" style="14" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="55.25" style="14" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="58.875" style="14" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="65.75" style="14" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="59" style="14" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="65.875" style="14" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="53.625" style="14" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="60.5" style="14" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="52.5" style="14" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="58.875" style="14" hidden="1" customWidth="1"/>
+    <col min="57" max="57" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="54.25" style="14" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="60.875" style="14" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="39.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="49.875" style="14" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="56.5" style="14" hidden="1" customWidth="1"/>
+    <col min="63" max="16384" width="37.5" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>144</v>
       </c>
@@ -1425,9 +1625,18 @@
       <c r="AX1" s="4"/>
       <c r="AY1" s="4"/>
       <c r="AZ1" s="4"/>
-      <c r="BA1" s="2"/>
+      <c r="BA1" s="4"/>
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="2"/>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>144</v>
       </c>
@@ -1476,115 +1685,142 @@
         <v>13</v>
       </c>
       <c r="R2" t="s">
+        <v>200</v>
+      </c>
+      <c r="S2" t="s">
+        <v>221</v>
+      </c>
+      <c r="T2" t="s">
+        <v>222</v>
+      </c>
+      <c r="U2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>15</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>16</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>17</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>18</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>19</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AD2" t="s">
         <v>131</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AE2" t="s">
         <v>132</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AF2" t="s">
         <v>133</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AG2" t="s">
         <v>23</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AH2" t="s">
         <v>24</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AI2" t="s">
         <v>25</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>224</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>226</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP2" t="s">
         <v>26</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AQ2" t="s">
         <v>27</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AR2" t="s">
         <v>28</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AS2" t="s">
         <v>29</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AT2" t="s">
         <v>30</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AU2" t="s">
         <v>31</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AV2" t="s">
         <v>32</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AW2" t="s">
         <v>33</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AX2" t="s">
         <v>34</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AY2" t="s">
         <v>35</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AZ2" t="s">
         <v>36</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="BA2" t="s">
         <v>37</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="BB2" t="s">
         <v>38</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="BC2" t="s">
         <v>39</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BD2" t="s">
         <v>40</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="BE2" t="s">
         <v>41</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="BF2" t="s">
         <v>42</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BG2" t="s">
         <v>43</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BH2" t="s">
         <v>44</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BI2" t="s">
         <v>45</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BJ2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>144</v>
       </c>
@@ -1640,8 +1876,17 @@
       <c r="AY3" s="3"/>
       <c r="AZ3"/>
       <c r="BA3"/>
+      <c r="BB3" s="3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1695,8 +1940,15 @@
       <c r="AY4" s="15"/>
       <c r="AZ4" s="15"/>
       <c r="BA4" s="15"/>
+      <c r="BB4" s="15"/>
+      <c r="BC4" s="15"/>
+      <c r="BD4" s="15"/>
+      <c r="BE4" s="15"/>
+      <c r="BF4" s="15"/>
+      <c r="BG4" s="15"/>
+      <c r="BH4" s="15"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>146</v>
       </c>
@@ -1725,65 +1977,76 @@
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16" t="s">
-        <v>59</v>
+        <v>201</v>
       </c>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
       <c r="U5" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="X5" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="Y5" s="16"/>
       <c r="Z5" s="16"/>
       <c r="AA5" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB5" s="16"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="16" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="AE5" s="16"/>
       <c r="AF5" s="16"/>
       <c r="AG5" s="16" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="AH5" s="16"/>
       <c r="AI5" s="16"/>
-      <c r="AJ5" s="16">
-        <v>50</v>
+      <c r="AJ5" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="AK5" s="16"/>
       <c r="AL5" s="16"/>
-      <c r="AM5" s="16">
-        <v>1300</v>
+      <c r="AM5" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="AN5" s="16"/>
       <c r="AO5" s="16"/>
       <c r="AP5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ5" s="16"/>
-      <c r="AR5" s="16"/>
-      <c r="AS5" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AT5" s="16"/>
-      <c r="AU5" s="16"/>
-      <c r="AV5" s="16" t="s">
-        <v>75</v>
+        <v>62</v>
+      </c>
+      <c r="AS5" s="16">
+        <v>50</v>
+      </c>
+      <c r="AV5" s="16">
+        <v>1300</v>
       </c>
       <c r="AW5" s="16"/>
       <c r="AX5" s="16"/>
-      <c r="AY5" s="16"/>
+      <c r="AY5" s="16" t="s">
+        <v>63</v>
+      </c>
       <c r="AZ5" s="16"/>
       <c r="BA5" s="16"/>
+      <c r="BB5" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC5" s="16"/>
+      <c r="BD5" s="16"/>
+      <c r="BE5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH5" s="16"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>146</v>
       </c>
@@ -1812,61 +2075,72 @@
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
       <c r="S6" s="16"/>
       <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16" t="s">
-        <v>72</v>
-      </c>
+      <c r="U6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="X6" s="16"/>
       <c r="Y6" s="16"/>
       <c r="Z6" s="16"/>
       <c r="AA6" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AB6" s="16"/>
       <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
+      <c r="AD6" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="AE6" s="16"/>
       <c r="AF6" s="16"/>
-      <c r="AG6" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="AG6" s="16"/>
       <c r="AH6" s="16"/>
       <c r="AI6" s="16"/>
-      <c r="AJ6" s="16">
-        <v>60</v>
+      <c r="AJ6" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="AK6" s="16"/>
       <c r="AL6" s="16"/>
-      <c r="AM6" s="16">
-        <v>1200</v>
+      <c r="AM6" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="AN6" s="16"/>
       <c r="AO6" s="16"/>
       <c r="AP6" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="AQ6" s="16"/>
-      <c r="AR6" s="16"/>
-      <c r="AS6" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AT6" s="16"/>
-      <c r="AU6" s="16"/>
-      <c r="AV6" s="16" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+      <c r="AS6" s="16">
+        <v>60</v>
+      </c>
+      <c r="AV6" s="16">
+        <v>1200</v>
       </c>
       <c r="AW6" s="16"/>
       <c r="AX6" s="16"/>
-      <c r="AY6" s="16"/>
+      <c r="AY6" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="AZ6" s="16"/>
       <c r="BA6" s="16"/>
+      <c r="BB6" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="BC6" s="16"/>
+      <c r="BD6" s="16"/>
+      <c r="BE6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="BF6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="BH6" s="16"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>146</v>
       </c>
@@ -1892,14 +2166,12 @@
       </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="16"/>
-      <c r="R7" s="16" t="s">
-        <v>78</v>
-      </c>
+      <c r="R7" s="16"/>
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
+      <c r="U7" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="X7" s="16"/>
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
@@ -1912,34 +2184,37 @@
       <c r="AG7" s="16"/>
       <c r="AH7" s="16"/>
       <c r="AI7" s="16"/>
-      <c r="AJ7" s="16">
-        <v>50</v>
-      </c>
+      <c r="AJ7" s="16"/>
       <c r="AK7" s="16"/>
       <c r="AL7" s="16"/>
-      <c r="AM7" s="16">
-        <v>650</v>
-      </c>
+      <c r="AM7" s="16"/>
       <c r="AN7" s="16"/>
       <c r="AO7" s="16"/>
-      <c r="AP7" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ7" s="16"/>
-      <c r="AR7" s="16"/>
-      <c r="AS7" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT7" s="16"/>
-      <c r="AU7" s="16"/>
-      <c r="AV7" s="16"/>
+      <c r="AP7" s="16"/>
+      <c r="AS7" s="16">
+        <v>50</v>
+      </c>
+      <c r="AV7" s="16">
+        <v>650</v>
+      </c>
       <c r="AW7" s="16"/>
       <c r="AX7" s="16"/>
-      <c r="AY7" s="16"/>
+      <c r="AY7" s="16" t="s">
+        <v>79</v>
+      </c>
       <c r="AZ7" s="16"/>
       <c r="BA7" s="16"/>
+      <c r="BB7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC7" s="16"/>
+      <c r="BD7" s="16"/>
+      <c r="BE7" s="16"/>
+      <c r="BF7" s="16"/>
+      <c r="BG7" s="16"/>
+      <c r="BH7" s="16"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>146</v>
       </c>
@@ -1965,25 +2240,23 @@
       </c>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
-      <c r="R8" s="16" t="s">
-        <v>85</v>
-      </c>
+      <c r="R8" s="16"/>
       <c r="S8" s="16"/>
       <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16" t="s">
-        <v>61</v>
-      </c>
+      <c r="U8" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="X8" s="16"/>
       <c r="Y8" s="16"/>
       <c r="Z8" s="16"/>
       <c r="AA8" s="16" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="AB8" s="16"/>
       <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
+      <c r="AD8" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="AE8" s="16"/>
       <c r="AF8" s="16"/>
       <c r="AG8" s="16"/>
@@ -1996,21 +2269,24 @@
       <c r="AN8" s="16"/>
       <c r="AO8" s="16"/>
       <c r="AP8" s="16"/>
-      <c r="AQ8" s="16"/>
-      <c r="AR8" s="16"/>
-      <c r="AS8" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT8" s="16"/>
-      <c r="AU8" s="16"/>
+      <c r="AS8" s="16"/>
       <c r="AV8" s="16"/>
       <c r="AW8" s="16"/>
       <c r="AX8" s="16"/>
       <c r="AY8" s="16"/>
       <c r="AZ8" s="16"/>
       <c r="BA8" s="16"/>
+      <c r="BB8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="BC8" s="16"/>
+      <c r="BD8" s="16"/>
+      <c r="BE8" s="16"/>
+      <c r="BF8" s="16"/>
+      <c r="BG8" s="16"/>
+      <c r="BH8" s="16"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>146</v>
       </c>
@@ -2032,23 +2308,21 @@
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
-      <c r="R9" s="16" t="s">
-        <v>89</v>
-      </c>
+      <c r="R9" s="16"/>
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
+      <c r="U9" s="16" t="s">
+        <v>89</v>
+      </c>
       <c r="X9" s="16"/>
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
-      <c r="AA9" s="16" t="s">
-        <v>90</v>
-      </c>
+      <c r="AA9" s="16"/>
       <c r="AB9" s="16"/>
       <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
+      <c r="AD9" s="16" t="s">
+        <v>90</v>
+      </c>
       <c r="AE9" s="16"/>
       <c r="AF9" s="16"/>
       <c r="AG9" s="16"/>
@@ -2060,22 +2334,25 @@
       <c r="AM9" s="16"/>
       <c r="AN9" s="16"/>
       <c r="AO9" s="16"/>
-      <c r="AP9" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ9" s="16"/>
-      <c r="AR9" s="16"/>
+      <c r="AP9" s="16"/>
       <c r="AS9" s="16"/>
-      <c r="AT9" s="16"/>
-      <c r="AU9" s="16"/>
       <c r="AV9" s="16"/>
       <c r="AW9" s="16"/>
       <c r="AX9" s="16"/>
-      <c r="AY9" s="16"/>
+      <c r="AY9" s="16" t="s">
+        <v>92</v>
+      </c>
       <c r="AZ9" s="16"/>
       <c r="BA9" s="16"/>
+      <c r="BB9" s="16"/>
+      <c r="BC9" s="16"/>
+      <c r="BD9" s="16"/>
+      <c r="BE9" s="16"/>
+      <c r="BF9" s="16"/>
+      <c r="BG9" s="16"/>
+      <c r="BH9" s="16"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>146</v>
       </c>
@@ -2099,8 +2376,6 @@
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
@@ -2120,8 +2395,6 @@
       <c r="AN10" s="16"/>
       <c r="AO10" s="16"/>
       <c r="AP10" s="16"/>
-      <c r="AQ10" s="16"/>
-      <c r="AR10" s="16"/>
       <c r="AS10" s="16"/>
       <c r="AT10" s="16"/>
       <c r="AU10" s="16"/>
@@ -2131,8 +2404,15 @@
       <c r="AY10" s="16"/>
       <c r="AZ10" s="16"/>
       <c r="BA10" s="16"/>
+      <c r="BB10" s="16"/>
+      <c r="BC10" s="16"/>
+      <c r="BD10" s="16"/>
+      <c r="BE10" s="16"/>
+      <c r="BF10" s="16"/>
+      <c r="BG10" s="16"/>
+      <c r="BH10" s="16"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2154,8 +2434,6 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
@@ -2175,8 +2453,6 @@
       <c r="AN11" s="15"/>
       <c r="AO11" s="15"/>
       <c r="AP11" s="15"/>
-      <c r="AQ11" s="15"/>
-      <c r="AR11" s="15"/>
       <c r="AS11" s="15"/>
       <c r="AT11" s="15"/>
       <c r="AU11" s="15"/>
@@ -2186,8 +2462,15 @@
       <c r="AY11" s="15"/>
       <c r="AZ11" s="15"/>
       <c r="BA11" s="15"/>
+      <c r="BB11" s="15"/>
+      <c r="BC11" s="15"/>
+      <c r="BD11" s="15"/>
+      <c r="BE11" s="15"/>
+      <c r="BF11" s="15"/>
+      <c r="BG11" s="15"/>
+      <c r="BH11" s="15"/>
     </row>
-    <row r="12" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>147</v>
       </c>
@@ -2220,67 +2503,76 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
       <c r="U12" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="X12" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="V12" s="17"/>
-      <c r="W12" s="17"/>
-      <c r="X12" s="17" t="s">
-        <v>135</v>
       </c>
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
       <c r="AA12" s="17" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="AB12" s="17"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="17" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="AE12" s="17"/>
       <c r="AF12" s="17"/>
       <c r="AG12" s="17" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="AH12" s="17"/>
       <c r="AI12" s="17"/>
       <c r="AJ12" s="17" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
       <c r="AK12" s="17"/>
       <c r="AL12" s="17"/>
       <c r="AM12" s="17" t="s">
-        <v>112</v>
+        <v>186</v>
       </c>
       <c r="AN12" s="17"/>
       <c r="AO12" s="17"/>
       <c r="AP12" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="AQ12" s="17"/>
-      <c r="AR12" s="17"/>
+        <v>110</v>
+      </c>
       <c r="AS12" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AT12" s="17"/>
       <c r="AU12" s="17"/>
       <c r="AV12" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AW12" s="17"/>
       <c r="AX12" s="17"/>
       <c r="AY12" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AZ12" s="17"/>
       <c r="BA12" s="17"/>
+      <c r="BB12" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="BC12" s="17"/>
+      <c r="BD12" s="17"/>
+      <c r="BE12" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF12" s="17"/>
+      <c r="BG12" s="17"/>
+      <c r="BH12" s="17" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="13" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>147</v>
       </c>
@@ -2313,67 +2605,76 @@
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="18" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="S13" s="18"/>
       <c r="T13" s="18"/>
       <c r="U13" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="X13" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18" t="s">
-        <v>101</v>
       </c>
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AE13" s="18"/>
       <c r="AF13" s="18"/>
       <c r="AG13" s="18" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="AH13" s="18"/>
       <c r="AI13" s="18"/>
       <c r="AJ13" s="18" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="AK13" s="18"/>
       <c r="AL13" s="18"/>
       <c r="AM13" s="18" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="AN13" s="18"/>
       <c r="AO13" s="18"/>
       <c r="AP13" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="AQ13" s="18"/>
-      <c r="AR13" s="18"/>
+        <v>137</v>
+      </c>
       <c r="AS13" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AT13" s="18"/>
       <c r="AU13" s="18"/>
       <c r="AV13" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AW13" s="18"/>
       <c r="AX13" s="18"/>
       <c r="AY13" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AZ13" s="18"/>
       <c r="BA13" s="18"/>
+      <c r="BB13" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC13" s="18"/>
+      <c r="BD13" s="18"/>
+      <c r="BE13" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF13" s="18"/>
+      <c r="BG13" s="18"/>
+      <c r="BH13" s="18" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="14" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>147</v>
       </c>
@@ -2397,12 +2698,12 @@
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
+      <c r="R14" s="19" t="s">
+        <v>203</v>
+      </c>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
       <c r="X14" s="19"/>
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
@@ -2412,43 +2713,52 @@
       <c r="AD14" s="19"/>
       <c r="AE14" s="19"/>
       <c r="AF14" s="19"/>
-      <c r="AG14" s="19" t="s">
-        <v>120</v>
-      </c>
+      <c r="AG14" s="19"/>
       <c r="AH14" s="19"/>
       <c r="AI14" s="19"/>
-      <c r="AJ14" s="19" t="s">
-        <v>121</v>
+      <c r="AJ14" s="46" t="s">
+        <v>181</v>
       </c>
       <c r="AK14" s="19"/>
       <c r="AL14" s="19"/>
-      <c r="AM14" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="AN14" s="19"/>
-      <c r="AO14" s="19"/>
+      <c r="AM14" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="AN14" s="46"/>
+      <c r="AO14" s="46"/>
       <c r="AP14" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="AQ14" s="19"/>
-      <c r="AR14" s="19"/>
+        <v>120</v>
+      </c>
       <c r="AS14" s="19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AT14" s="19"/>
       <c r="AU14" s="19"/>
       <c r="AV14" s="19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AW14" s="19"/>
       <c r="AX14" s="19"/>
       <c r="AY14" s="19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AZ14" s="19"/>
       <c r="BA14" s="19"/>
+      <c r="BB14" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="BC14" s="19"/>
+      <c r="BD14" s="19"/>
+      <c r="BE14" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF14" s="19"/>
+      <c r="BG14" s="19"/>
+      <c r="BH14" s="19" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="15" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>147</v>
       </c>
@@ -2478,56 +2788,63 @@
       <c r="S15" s="21"/>
       <c r="T15" s="21"/>
       <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21" t="s">
-        <v>117</v>
-      </c>
+      <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
       <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
+      <c r="AA15" s="21" t="s">
+        <v>117</v>
+      </c>
       <c r="AB15" s="21"/>
       <c r="AC15" s="21"/>
       <c r="AD15" s="21"/>
       <c r="AE15" s="21"/>
       <c r="AF15" s="21"/>
-      <c r="AG15" s="21" t="s">
-        <v>117</v>
-      </c>
+      <c r="AG15" s="21"/>
       <c r="AH15" s="21"/>
       <c r="AI15" s="21"/>
       <c r="AJ15" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AK15" s="21"/>
       <c r="AL15" s="21"/>
       <c r="AM15" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AN15" s="21"/>
       <c r="AO15" s="21"/>
       <c r="AP15" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="AQ15" s="21"/>
-      <c r="AR15" s="21"/>
       <c r="AS15" s="21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AT15" s="21"/>
       <c r="AU15" s="21"/>
       <c r="AV15" s="21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AW15" s="21"/>
       <c r="AX15" s="21"/>
       <c r="AY15" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="AZ15" s="19"/>
-      <c r="BA15" s="19"/>
+      <c r="AZ15" s="21"/>
+      <c r="BA15" s="21"/>
+      <c r="BB15" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC15" s="21"/>
+      <c r="BD15" s="21"/>
+      <c r="BE15" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF15" s="21"/>
+      <c r="BG15" s="21"/>
+      <c r="BH15" s="21" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="16" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>153</v>
       </c>
@@ -2555,14 +2872,12 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
-      <c r="R16" s="45" t="s">
+      <c r="R16" s="20"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="S16" s="20"/>
-      <c r="T16" s="20"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="20"/>
       <c r="X16" s="20"/>
       <c r="Y16" s="20"/>
       <c r="Z16" s="20"/>
@@ -2578,25 +2893,32 @@
       <c r="AJ16" s="20"/>
       <c r="AK16" s="20"/>
       <c r="AL16" s="20"/>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="AN16" s="20"/>
       <c r="AO16" s="20"/>
-      <c r="AP16" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="AQ16" s="20"/>
-      <c r="AR16" s="20"/>
+      <c r="AP16" s="20"/>
       <c r="AS16" s="20"/>
       <c r="AT16" s="20"/>
       <c r="AU16" s="20"/>
       <c r="AV16" s="20"/>
       <c r="AW16" s="20"/>
       <c r="AX16" s="20"/>
-      <c r="AY16" s="20"/>
+      <c r="AY16" s="45" t="s">
+        <v>175</v>
+      </c>
       <c r="AZ16" s="20"/>
       <c r="BA16" s="20"/>
+      <c r="BB16" s="20"/>
+      <c r="BC16" s="20"/>
+      <c r="BD16" s="20"/>
+      <c r="BE16" s="20"/>
+      <c r="BF16" s="20"/>
+      <c r="BG16" s="20"/>
+      <c r="BH16" s="20"/>
     </row>
-    <row r="17" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>153</v>
       </c>
@@ -2622,20 +2944,18 @@
       <c r="S17" s="21"/>
       <c r="T17" s="21"/>
       <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
       <c r="X17" s="21"/>
       <c r="Y17" s="21"/>
       <c r="Z17" s="21"/>
       <c r="AA17" s="21"/>
       <c r="AB17" s="21"/>
       <c r="AC17" s="21"/>
-      <c r="AD17" s="38" t="s">
-        <v>171</v>
-      </c>
+      <c r="AD17" s="21"/>
       <c r="AE17" s="21"/>
       <c r="AF17" s="21"/>
-      <c r="AG17" s="21"/>
+      <c r="AG17" s="38" t="s">
+        <v>171</v>
+      </c>
       <c r="AH17" s="21"/>
       <c r="AI17" s="21"/>
       <c r="AJ17" s="21"/>
@@ -2645,8 +2965,6 @@
       <c r="AN17" s="21"/>
       <c r="AO17" s="21"/>
       <c r="AP17" s="21"/>
-      <c r="AQ17" s="21"/>
-      <c r="AR17" s="21"/>
       <c r="AS17" s="21"/>
       <c r="AT17" s="21"/>
       <c r="AU17" s="21"/>
@@ -2656,8 +2974,15 @@
       <c r="AY17" s="21"/>
       <c r="AZ17" s="21"/>
       <c r="BA17" s="21"/>
+      <c r="BB17" s="21"/>
+      <c r="BC17" s="21"/>
+      <c r="BD17" s="21"/>
+      <c r="BE17" s="21"/>
+      <c r="BF17" s="21"/>
+      <c r="BG17" s="21"/>
+      <c r="BH17" s="21"/>
     </row>
-    <row r="18" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>156</v>
       </c>
@@ -2683,22 +3008,20 @@
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
-      <c r="R18" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="R18" s="19"/>
       <c r="S18" s="19"/>
       <c r="T18" s="19"/>
       <c r="U18" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="X18" s="19" t="s">
         <v>127</v>
-      </c>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19" t="s">
-        <v>134</v>
       </c>
       <c r="Y18" s="19"/>
       <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
+      <c r="AA18" s="19" t="s">
+        <v>134</v>
+      </c>
       <c r="AB18" s="19"/>
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
@@ -2714,8 +3037,6 @@
       <c r="AN18" s="19"/>
       <c r="AO18" s="19"/>
       <c r="AP18" s="19"/>
-      <c r="AQ18" s="19"/>
-      <c r="AR18" s="19"/>
       <c r="AS18" s="19"/>
       <c r="AT18" s="19"/>
       <c r="AU18" s="19"/>
@@ -2725,8 +3046,15 @@
       <c r="AY18" s="19"/>
       <c r="AZ18" s="19"/>
       <c r="BA18" s="19"/>
+      <c r="BB18" s="19"/>
+      <c r="BC18" s="19"/>
+      <c r="BD18" s="19"/>
+      <c r="BE18" s="19"/>
+      <c r="BF18" s="19"/>
+      <c r="BG18" s="19"/>
+      <c r="BH18" s="19"/>
     </row>
-    <row r="19" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>156</v>
       </c>
@@ -2756,14 +3084,12 @@
       <c r="S19" s="19"/>
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="20" t="s">
-        <v>128</v>
-      </c>
+      <c r="X19" s="19"/>
       <c r="Y19" s="19"/>
       <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
+      <c r="AA19" s="20" t="s">
+        <v>128</v>
+      </c>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>
@@ -2779,8 +3105,6 @@
       <c r="AN19" s="19"/>
       <c r="AO19" s="19"/>
       <c r="AP19" s="19"/>
-      <c r="AQ19" s="19"/>
-      <c r="AR19" s="19"/>
       <c r="AS19" s="19"/>
       <c r="AT19" s="19"/>
       <c r="AU19" s="19"/>
@@ -2790,8 +3114,15 @@
       <c r="AY19" s="19"/>
       <c r="AZ19" s="19"/>
       <c r="BA19" s="19"/>
+      <c r="BB19" s="19"/>
+      <c r="BC19" s="19"/>
+      <c r="BD19" s="19"/>
+      <c r="BE19" s="19"/>
+      <c r="BF19" s="19"/>
+      <c r="BG19" s="19"/>
+      <c r="BH19" s="19"/>
     </row>
-    <row r="20" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>156</v>
       </c>
@@ -2817,8 +3148,6 @@
       <c r="S20" s="19"/>
       <c r="T20" s="19"/>
       <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="19"/>
       <c r="X20" s="19"/>
       <c r="Y20" s="19"/>
       <c r="Z20" s="19"/>
@@ -2838,8 +3167,6 @@
       <c r="AN20" s="19"/>
       <c r="AO20" s="19"/>
       <c r="AP20" s="19"/>
-      <c r="AQ20" s="19"/>
-      <c r="AR20" s="19"/>
       <c r="AS20" s="19"/>
       <c r="AT20" s="19"/>
       <c r="AU20" s="19"/>
@@ -2849,8 +3176,15 @@
       <c r="AY20" s="19"/>
       <c r="AZ20" s="19"/>
       <c r="BA20" s="19"/>
+      <c r="BB20" s="19"/>
+      <c r="BC20" s="19"/>
+      <c r="BD20" s="19"/>
+      <c r="BE20" s="19"/>
+      <c r="BF20" s="19"/>
+      <c r="BG20" s="19"/>
+      <c r="BH20" s="19"/>
     </row>
-    <row r="21" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>156</v>
       </c>
@@ -2883,11 +3217,7 @@
       <c r="R21" s="19"/>
       <c r="S21" s="19"/>
       <c r="T21" s="19"/>
-      <c r="U21" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
+      <c r="U21" s="19"/>
       <c r="X21" s="44" t="s">
         <v>173</v>
       </c>
@@ -2908,24 +3238,26 @@
       </c>
       <c r="AH21" s="19"/>
       <c r="AI21" s="19"/>
-      <c r="AJ21" s="44" t="s">
-        <v>173</v>
-      </c>
+      <c r="AJ21" s="47"/>
       <c r="AK21" s="19"/>
       <c r="AL21" s="19"/>
       <c r="AM21" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="AN21" s="19"/>
-      <c r="AO21" s="19"/>
-      <c r="AP21" s="19"/>
-      <c r="AQ21" s="19"/>
-      <c r="AR21" s="19"/>
+      <c r="AN21" s="44"/>
+      <c r="AO21" s="44"/>
+      <c r="AP21" s="44" t="s">
+        <v>173</v>
+      </c>
       <c r="AS21" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="AT21" s="19"/>
-      <c r="AU21" s="19"/>
+      <c r="AT21" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="AU21" s="44" t="s">
+        <v>173</v>
+      </c>
       <c r="AV21" s="44" t="s">
         <v>173</v>
       </c>
@@ -2936,8 +3268,25 @@
       </c>
       <c r="AZ21" s="19"/>
       <c r="BA21" s="19"/>
+      <c r="BB21" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="BC21" s="19"/>
+      <c r="BD21" s="19"/>
+      <c r="BE21" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="BF21" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="BG21" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="BH21" s="44" t="s">
+        <v>173</v>
+      </c>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2959,8 +3308,6 @@
       <c r="S22" s="22"/>
       <c r="T22" s="22"/>
       <c r="U22" s="22"/>
-      <c r="V22" s="22"/>
-      <c r="W22" s="22"/>
       <c r="X22" s="22"/>
       <c r="Y22" s="22"/>
       <c r="Z22" s="22"/>
@@ -2991,8 +3338,15 @@
       <c r="AY22" s="22"/>
       <c r="AZ22" s="22"/>
       <c r="BA22" s="22"/>
+      <c r="BB22" s="22"/>
+      <c r="BC22" s="22"/>
+      <c r="BD22" s="22"/>
+      <c r="BE22" s="22"/>
+      <c r="BF22" s="22"/>
+      <c r="BG22" s="22"/>
+      <c r="BH22" s="22"/>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
@@ -3014,8 +3368,6 @@
       <c r="S23" s="22"/>
       <c r="T23" s="22"/>
       <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
-      <c r="W23" s="22"/>
       <c r="X23" s="22"/>
       <c r="Y23" s="22"/>
       <c r="Z23" s="22"/>
@@ -3046,8 +3398,15 @@
       <c r="AY23" s="22"/>
       <c r="AZ23" s="22"/>
       <c r="BA23" s="22"/>
+      <c r="BB23" s="22"/>
+      <c r="BC23" s="22"/>
+      <c r="BD23" s="22"/>
+      <c r="BE23" s="22"/>
+      <c r="BF23" s="22"/>
+      <c r="BG23" s="22"/>
+      <c r="BH23" s="22"/>
     </row>
-    <row r="24" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:60" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>54</v>
       </c>
@@ -3058,32 +3417,40 @@
         <v>162</v>
       </c>
       <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="E24" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" s="46"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
+      <c r="O24" s="48" t="s">
+        <v>190</v>
+      </c>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
+      <c r="R24" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="S24" s="50"/>
       <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-      <c r="W24" s="19"/>
+      <c r="U24" s="50" t="s">
+        <v>194</v>
+      </c>
       <c r="X24" s="19"/>
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
-      <c r="AA24" s="19"/>
+      <c r="AA24" s="46"/>
       <c r="AB24" s="19"/>
       <c r="AC24" s="19"/>
-      <c r="AD24" s="19"/>
+      <c r="AD24" s="48" t="s">
+        <v>198</v>
+      </c>
       <c r="AE24" s="19"/>
       <c r="AF24" s="19"/>
       <c r="AG24" s="19"/>
@@ -3095,20 +3462,49 @@
       <c r="AM24" s="19"/>
       <c r="AN24" s="19"/>
       <c r="AO24" s="19"/>
-      <c r="AP24" s="19"/>
+      <c r="AP24" s="50" t="s">
+        <v>208</v>
+      </c>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="19"/>
-      <c r="AS24" s="19"/>
-      <c r="AT24" s="19"/>
-      <c r="AU24" s="19"/>
-      <c r="AV24" s="19"/>
+      <c r="AS24" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="AT24" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="AU24" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="AV24" s="48" t="s">
+        <v>210</v>
+      </c>
       <c r="AW24" s="19"/>
       <c r="AX24" s="19"/>
-      <c r="AY24" s="19"/>
+      <c r="AY24" s="50" t="s">
+        <v>213</v>
+      </c>
       <c r="AZ24" s="19"/>
       <c r="BA24" s="19"/>
+      <c r="BB24" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC24" s="19"/>
+      <c r="BD24" s="19"/>
+      <c r="BE24" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="BF24" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="BG24" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="BH24" s="50" t="s">
+        <v>217</v>
+      </c>
     </row>
-    <row r="25" spans="1:53" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:60" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>54</v>
       </c>
@@ -3119,32 +3515,40 @@
         <v>164</v>
       </c>
       <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="E25" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="46"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
+      <c r="O25" s="48" t="s">
+        <v>191</v>
+      </c>
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
+      <c r="R25" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="S25" s="50"/>
       <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
+      <c r="U25" s="50" t="s">
+        <v>195</v>
+      </c>
       <c r="X25" s="19"/>
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
+      <c r="AA25" s="46"/>
       <c r="AB25" s="19"/>
       <c r="AC25" s="19"/>
-      <c r="AD25" s="19"/>
+      <c r="AD25" s="48" t="s">
+        <v>199</v>
+      </c>
       <c r="AE25" s="19"/>
       <c r="AF25" s="19"/>
       <c r="AG25" s="19"/>
@@ -3156,20 +3560,49 @@
       <c r="AM25" s="19"/>
       <c r="AN25" s="19"/>
       <c r="AO25" s="19"/>
-      <c r="AP25" s="19"/>
+      <c r="AP25" s="50" t="s">
+        <v>209</v>
+      </c>
       <c r="AQ25" s="19"/>
       <c r="AR25" s="19"/>
-      <c r="AS25" s="19"/>
-      <c r="AT25" s="19"/>
-      <c r="AU25" s="19"/>
-      <c r="AV25" s="19"/>
+      <c r="AS25" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT25" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="AU25" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="AV25" s="48" t="s">
+        <v>211</v>
+      </c>
       <c r="AW25" s="19"/>
       <c r="AX25" s="19"/>
-      <c r="AY25" s="19"/>
+      <c r="AY25" s="50" t="s">
+        <v>214</v>
+      </c>
       <c r="AZ25" s="19"/>
       <c r="BA25" s="19"/>
+      <c r="BB25" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC25" s="19"/>
+      <c r="BD25" s="19"/>
+      <c r="BE25" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="BF25" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="BG25" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="BH25" s="50" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="26" spans="1:53" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:60" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>54</v>
       </c>
@@ -3180,32 +3613,40 @@
         <v>166</v>
       </c>
       <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="E26" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="46"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
+      <c r="O26" s="48" t="s">
+        <v>192</v>
+      </c>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
+      <c r="R26" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="S26" s="50"/>
       <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="19"/>
+      <c r="U26" s="50" t="s">
+        <v>196</v>
+      </c>
       <c r="X26" s="19"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
-      <c r="AA26" s="19"/>
+      <c r="AA26" s="46"/>
       <c r="AB26" s="19"/>
       <c r="AC26" s="19"/>
-      <c r="AD26" s="19"/>
+      <c r="AD26" s="48" t="s">
+        <v>196</v>
+      </c>
       <c r="AE26" s="19"/>
       <c r="AF26" s="19"/>
       <c r="AG26" s="19"/>
@@ -3217,20 +3658,49 @@
       <c r="AM26" s="19"/>
       <c r="AN26" s="19"/>
       <c r="AO26" s="19"/>
-      <c r="AP26" s="19"/>
+      <c r="AP26" s="50" t="s">
+        <v>196</v>
+      </c>
       <c r="AQ26" s="19"/>
       <c r="AR26" s="19"/>
-      <c r="AS26" s="19"/>
-      <c r="AT26" s="19"/>
-      <c r="AU26" s="19"/>
-      <c r="AV26" s="19"/>
+      <c r="AS26" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT26" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="AU26" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="AV26" s="48" t="s">
+        <v>196</v>
+      </c>
       <c r="AW26" s="19"/>
       <c r="AX26" s="19"/>
-      <c r="AY26" s="19"/>
+      <c r="AY26" s="50" t="s">
+        <v>196</v>
+      </c>
       <c r="AZ26" s="19"/>
       <c r="BA26" s="19"/>
+      <c r="BB26" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="BC26" s="19"/>
+      <c r="BD26" s="19"/>
+      <c r="BE26" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="BF26" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="BG26" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="BH26" s="50" t="s">
+        <v>196</v>
+      </c>
     </row>
-    <row r="27" spans="1:53" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:60" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>54</v>
       </c>
@@ -3241,32 +3711,40 @@
         <v>168</v>
       </c>
       <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
+      <c r="E27" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="46"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
+      <c r="O27" s="48" t="s">
+        <v>193</v>
+      </c>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
+      <c r="R27" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="S27" s="50"/>
       <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19"/>
-      <c r="W27" s="19"/>
+      <c r="U27" s="50" t="s">
+        <v>197</v>
+      </c>
       <c r="X27" s="19"/>
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
-      <c r="AA27" s="19"/>
+      <c r="AA27" s="46"/>
       <c r="AB27" s="19"/>
       <c r="AC27" s="19"/>
-      <c r="AD27" s="19"/>
+      <c r="AD27" s="48" t="s">
+        <v>197</v>
+      </c>
       <c r="AE27" s="19"/>
       <c r="AF27" s="19"/>
       <c r="AG27" s="19"/>
@@ -3278,20 +3756,49 @@
       <c r="AM27" s="19"/>
       <c r="AN27" s="19"/>
       <c r="AO27" s="19"/>
-      <c r="AP27" s="19"/>
+      <c r="AP27" s="50" t="s">
+        <v>197</v>
+      </c>
       <c r="AQ27" s="19"/>
       <c r="AR27" s="19"/>
-      <c r="AS27" s="19"/>
-      <c r="AT27" s="19"/>
-      <c r="AU27" s="19"/>
-      <c r="AV27" s="19"/>
+      <c r="AS27" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="AT27" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU27" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="AV27" s="48" t="s">
+        <v>212</v>
+      </c>
       <c r="AW27" s="19"/>
       <c r="AX27" s="19"/>
-      <c r="AY27" s="19"/>
+      <c r="AY27" s="50" t="s">
+        <v>197</v>
+      </c>
       <c r="AZ27" s="19"/>
       <c r="BA27" s="19"/>
+      <c r="BB27" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="BC27" s="19"/>
+      <c r="BD27" s="19"/>
+      <c r="BE27" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="BF27" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="BG27" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="BH27" s="50" t="s">
+        <v>197</v>
+      </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>54</v>
       </c>
@@ -3303,10 +3810,10 @@
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
       <c r="L28" s="19"/>
@@ -3319,8 +3826,6 @@
       <c r="S28" s="19"/>
       <c r="T28" s="19"/>
       <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
       <c r="X28" s="19"/>
       <c r="Y28" s="19"/>
       <c r="Z28" s="19"/>
@@ -3351,8 +3856,15 @@
       <c r="AY28" s="19"/>
       <c r="AZ28" s="19"/>
       <c r="BA28" s="19"/>
+      <c r="BB28" s="19"/>
+      <c r="BC28" s="19"/>
+      <c r="BD28" s="19"/>
+      <c r="BE28" s="19"/>
+      <c r="BF28" s="19"/>
+      <c r="BG28" s="19"/>
+      <c r="BH28" s="19"/>
     </row>
-    <row r="29" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:60" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -3380,8 +3892,6 @@
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
       <c r="U29" s="21"/>
-      <c r="V29" s="21"/>
-      <c r="W29" s="21"/>
       <c r="X29" s="21"/>
       <c r="Y29" s="21"/>
       <c r="Z29" s="21"/>
@@ -3412,8 +3922,15 @@
       <c r="AY29" s="21"/>
       <c r="AZ29" s="21"/>
       <c r="BA29" s="21"/>
+      <c r="BB29" s="21"/>
+      <c r="BC29" s="21"/>
+      <c r="BD29" s="21"/>
+      <c r="BE29" s="21"/>
+      <c r="BF29" s="21"/>
+      <c r="BG29" s="21"/>
+      <c r="BH29" s="21"/>
     </row>
-    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="37"/>
       <c r="C30" s="37"/>
@@ -3435,8 +3952,6 @@
       <c r="S30" s="15"/>
       <c r="T30" s="15"/>
       <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
       <c r="X30" s="15"/>
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
@@ -3467,23 +3982,32 @@
       <c r="AY30" s="15"/>
       <c r="AZ30" s="15"/>
       <c r="BA30" s="15"/>
+      <c r="BB30" s="15"/>
+      <c r="BC30" s="15"/>
+      <c r="BD30" s="15"/>
+      <c r="BE30" s="15"/>
+      <c r="BF30" s="15"/>
+      <c r="BG30" s="15"/>
+      <c r="BH30" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="U18" r:id="rId1" display="http://purl.obolibrary.org/obo/OBI_0000555" xr:uid="{0F4407F2-2D05-9749-8F4A-097A23356DC6}"/>
-    <hyperlink ref="AS14" r:id="rId2" xr:uid="{E0715D4C-5FD8-164C-8257-A0A0BB5625EF}"/>
-    <hyperlink ref="AY14" r:id="rId3" xr:uid="{1118F33C-B27D-7644-9A23-642B8181A934}"/>
-    <hyperlink ref="AP14" r:id="rId4" xr:uid="{5C10F8DF-4069-1E45-BEC7-4ABBE409B1F1}"/>
-    <hyperlink ref="AM14" r:id="rId5" xr:uid="{7B350DBC-6C76-794D-85BA-8624BC573C2E}"/>
-    <hyperlink ref="AJ14" r:id="rId6" xr:uid="{B99BA9A9-46C5-1B48-AE21-57ECD9E93AB8}"/>
-    <hyperlink ref="AG14" r:id="rId7" xr:uid="{024CDF76-7112-4C41-944B-513D5B8E37D7}"/>
-    <hyperlink ref="AV14" r:id="rId8" xr:uid="{41401BAE-D4B2-034D-BAB8-7E0B9A642874}"/>
-    <hyperlink ref="O19" r:id="rId9" xr:uid="{BB9B92EF-9404-474F-8537-A82CE94282EE}"/>
-    <hyperlink ref="AD17" r:id="rId10" xr:uid="{EFE5B530-29C3-0D4D-A786-0D28594D7F0B}"/>
+    <hyperlink ref="X18" r:id="rId1" display="http://purl.obolibrary.org/obo/OBI_0000555" xr:uid="{0F4407F2-2D05-9749-8F4A-097A23356DC6}"/>
+    <hyperlink ref="BB14" r:id="rId2" xr:uid="{E0715D4C-5FD8-164C-8257-A0A0BB5625EF}"/>
+    <hyperlink ref="BH14" r:id="rId3" xr:uid="{1118F33C-B27D-7644-9A23-642B8181A934}"/>
+    <hyperlink ref="AY14" r:id="rId4" xr:uid="{5C10F8DF-4069-1E45-BEC7-4ABBE409B1F1}"/>
+    <hyperlink ref="AV14" r:id="rId5" xr:uid="{7B350DBC-6C76-794D-85BA-8624BC573C2E}"/>
+    <hyperlink ref="BE14" r:id="rId6" xr:uid="{41401BAE-D4B2-034D-BAB8-7E0B9A642874}"/>
+    <hyperlink ref="O19" r:id="rId7" xr:uid="{BB9B92EF-9404-474F-8537-A82CE94282EE}"/>
+    <hyperlink ref="AG17" r:id="rId8" xr:uid="{EFE5B530-29C3-0D4D-A786-0D28594D7F0B}"/>
+    <hyperlink ref="AS14" r:id="rId9" xr:uid="{B99BA9A9-46C5-1B48-AE21-57ECD9E93AB8}"/>
+    <hyperlink ref="AP14" r:id="rId10" xr:uid="{08527ECA-BE56-4143-8267-4AB85742F4F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>